<commit_message>
Tweak chart ready for modelling-regional-occurrences
</commit_message>
<xml_diff>
--- a/data/phe-surveillance/xlsx/explore_phe_delays.xlsx
+++ b/data/phe-surveillance/xlsx/explore_phe_delays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\covid-stats\data\phe-surveillance\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B583D2-4B39-4DA5-A527-BCAF66DB058C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42DDA75-32FB-4567-AB13-2FE80E45A418}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{CF9BCB3E-FB85-4E8E-90AD-6AD45E084C0E}"/>
   </bookViews>
@@ -349,6 +349,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Effect of Registration Delays on PHE Surveillance Reports</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -385,15 +410,15 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Figure 49. Daily excess deaths'!$C$8</c:f>
+              <c:f>'Figure 49. Daily excess deaths'!$H$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Delayed corrected deaths </c:v>
+                  <c:v>29/12/2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1584,2312 +1609,6 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Figure 49. Daily excess deaths'!$C$9:$C$372</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="364"/>
-                <c:pt idx="0">
-                  <c:v>1622</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1733</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1701</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1617</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1584</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1640</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1621</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1621</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1643</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1557</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1551</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1635</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1578</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1545</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1563</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1559</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1544</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1419</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1362</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1438</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1554</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1513</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1463</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1448</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1437</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1492</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1494</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1434</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1415</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1482</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1553</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1401</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1436</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1351</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1382</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1442</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1457</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1511</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1442</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>1488</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1544</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>1324</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>1437</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>1473</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1416</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>1502</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>1459</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>1410</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>1402</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>1430</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>1485</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>1447</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>1490</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>1353</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>1443</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>1479</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>1380</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>1369</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>1455</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>1513</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>1439</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>1560</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>1491</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>1412</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>1354</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>1507</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>1427</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>1442</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>1427</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>1496</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>1498</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>1397</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>1401</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>1401</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>1450</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>1516</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>1539</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>1564</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>1557</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>1614</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>1636</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>1677</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>1768</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>1803</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>1906</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>1964</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>2063</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>2122</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>1981</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>2313</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>2423</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>2553</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>2665</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>2666</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>2876</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>2889</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>2872</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>2895</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>3088</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>2980</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>2966</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>2963</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>2973</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>2686</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>2617</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>2755</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>2829</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>2733</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>2624</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>2595</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>2554</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>2480</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>2452</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>2367</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>2372</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>2267</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>2178</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>2217</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>2056</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>1958</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>2024</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>1926</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>1851</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>1847</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>1779</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>1759</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>1805</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>1769</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>1738</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>1630</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>1485</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>1547</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>1584</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>1507</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>1613</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>1524</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>1534</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>1560</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>1550</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>1484</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>1517</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>1383</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>1341</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>1278</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>1335</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>1434</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>1381</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>1316</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>1359</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>1286</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>1277</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>1352</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>1400</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>1271</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>1298</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>1295</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>1205</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>1236</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>1323</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>1261</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>1247</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>1204</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>1205</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>1258</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>1219</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>1237</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>1227</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>1224</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>1171</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>1132</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>1212</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>1158</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>1201</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>1249</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>1302</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>1371</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>1352</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>1205</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>1089</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>1116</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>1158</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>1167</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>1137</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>1149</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>1100</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>1108</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>1097</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>1088</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>1175</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>1234</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>1130</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>1143</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>1122</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>1192</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>1142</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>1125</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>1148</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>1231</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>1234</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>1140</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>1119</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>1162</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>1174</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>1222</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>1227</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>1147</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>1094</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>1152</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>1117</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>1113</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>1150</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>1314</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>1211</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>1093</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>1141</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>1128</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>1152</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>1212</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>1234</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>1252</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>1178</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>1253</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>1461</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>1529</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>1375</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>1185</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>1174</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>1171</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>1131</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>1156</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>1115</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>1141</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>1077</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>1084</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>1068</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>1110</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>1227</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>1092</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>1047</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>1194</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>1121</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>1137</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>1206</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>1130</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>1135</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>1231</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>1250</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>1175</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>1208</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>1214</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>1264</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>1235</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>1058</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>1106</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>1199</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>1151</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>1251</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>1279</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>1240</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>1163</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>1203</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>1226</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>1187</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>1263</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>1226</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>1224</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>1211</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>1213</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>1209</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>1313</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>1284</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>1272</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>1222</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>1269</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>1316</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>1329</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>1348</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>1326</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>1273</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>1291</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>1351</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>1249</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>1227</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>1301</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>1287</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>1273</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>1369</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>1359</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>1349</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>1403</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>1374</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>1336</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>1442</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>1551</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>1370</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>1317</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>1355</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>1429</c:v>
-                </c:pt>
-                <c:pt idx="299">
-                  <c:v>1384</c:v>
-                </c:pt>
-                <c:pt idx="300">
-                  <c:v>1443</c:v>
-                </c:pt>
-                <c:pt idx="301">
-                  <c:v>1416</c:v>
-                </c:pt>
-                <c:pt idx="302">
-                  <c:v>1492</c:v>
-                </c:pt>
-                <c:pt idx="303">
-                  <c:v>1473</c:v>
-                </c:pt>
-                <c:pt idx="304">
-                  <c:v>1460</c:v>
-                </c:pt>
-                <c:pt idx="305">
-                  <c:v>1472</c:v>
-                </c:pt>
-                <c:pt idx="306">
-                  <c:v>1508</c:v>
-                </c:pt>
-                <c:pt idx="307">
-                  <c:v>1457</c:v>
-                </c:pt>
-                <c:pt idx="308">
-                  <c:v>1381</c:v>
-                </c:pt>
-                <c:pt idx="309">
-                  <c:v>1489</c:v>
-                </c:pt>
-                <c:pt idx="310">
-                  <c:v>1546</c:v>
-                </c:pt>
-                <c:pt idx="311">
-                  <c:v>1509</c:v>
-                </c:pt>
-                <c:pt idx="312">
-                  <c:v>1591</c:v>
-                </c:pt>
-                <c:pt idx="313">
-                  <c:v>1641</c:v>
-                </c:pt>
-                <c:pt idx="314">
-                  <c:v>1483</c:v>
-                </c:pt>
-                <c:pt idx="315">
-                  <c:v>1497</c:v>
-                </c:pt>
-                <c:pt idx="316">
-                  <c:v>1539</c:v>
-                </c:pt>
-                <c:pt idx="317">
-                  <c:v>1520</c:v>
-                </c:pt>
-                <c:pt idx="318">
-                  <c:v>1534</c:v>
-                </c:pt>
-                <c:pt idx="319">
-                  <c:v>1524</c:v>
-                </c:pt>
-                <c:pt idx="320">
-                  <c:v>1474</c:v>
-                </c:pt>
-                <c:pt idx="321">
-                  <c:v>1543</c:v>
-                </c:pt>
-                <c:pt idx="322">
-                  <c:v>1602</c:v>
-                </c:pt>
-                <c:pt idx="323">
-                  <c:v>1473</c:v>
-                </c:pt>
-                <c:pt idx="324">
-                  <c:v>1571</c:v>
-                </c:pt>
-                <c:pt idx="325">
-                  <c:v>1596</c:v>
-                </c:pt>
-                <c:pt idx="326">
-                  <c:v>1518</c:v>
-                </c:pt>
-                <c:pt idx="327">
-                  <c:v>1526</c:v>
-                </c:pt>
-                <c:pt idx="328">
-                  <c:v>1580</c:v>
-                </c:pt>
-                <c:pt idx="329">
-                  <c:v>1626</c:v>
-                </c:pt>
-                <c:pt idx="330">
-                  <c:v>1464</c:v>
-                </c:pt>
-                <c:pt idx="331">
-                  <c:v>1498</c:v>
-                </c:pt>
-                <c:pt idx="332">
-                  <c:v>1543</c:v>
-                </c:pt>
-                <c:pt idx="333">
-                  <c:v>1576</c:v>
-                </c:pt>
-                <c:pt idx="334">
-                  <c:v>1584</c:v>
-                </c:pt>
-                <c:pt idx="335">
-                  <c:v>1480</c:v>
-                </c:pt>
-                <c:pt idx="336">
-                  <c:v>1535</c:v>
-                </c:pt>
-                <c:pt idx="337">
-                  <c:v>1560</c:v>
-                </c:pt>
-                <c:pt idx="338">
-                  <c:v>1570</c:v>
-                </c:pt>
-                <c:pt idx="339">
-                  <c:v>1537</c:v>
-                </c:pt>
-                <c:pt idx="340">
-                  <c:v>1535</c:v>
-                </c:pt>
-                <c:pt idx="341">
-                  <c:v>1535</c:v>
-                </c:pt>
-                <c:pt idx="342">
-                  <c:v>1598</c:v>
-                </c:pt>
-                <c:pt idx="343">
-                  <c:v>1609</c:v>
-                </c:pt>
-                <c:pt idx="344">
-                  <c:v>1644</c:v>
-                </c:pt>
-                <c:pt idx="345">
-                  <c:v>1632</c:v>
-                </c:pt>
-                <c:pt idx="346">
-                  <c:v>1548</c:v>
-                </c:pt>
-                <c:pt idx="347">
-                  <c:v>1462</c:v>
-                </c:pt>
-                <c:pt idx="348">
-                  <c:v>1572</c:v>
-                </c:pt>
-                <c:pt idx="349">
-                  <c:v>1477</c:v>
-                </c:pt>
-                <c:pt idx="350">
-                  <c:v>1415</c:v>
-                </c:pt>
-                <c:pt idx="351">
-                  <c:v>1506</c:v>
-                </c:pt>
-                <c:pt idx="352">
-                  <c:v>1447</c:v>
-                </c:pt>
-                <c:pt idx="353">
-                  <c:v>1333</c:v>
-                </c:pt>
-                <c:pt idx="354">
-                  <c:v>1231</c:v>
-                </c:pt>
-                <c:pt idx="355">
-                  <c:v>1241</c:v>
-                </c:pt>
-                <c:pt idx="356">
-                  <c:v>1517</c:v>
-                </c:pt>
-                <c:pt idx="357">
-                  <c:v>1544</c:v>
-                </c:pt>
-                <c:pt idx="358">
-                  <c:v>1358</c:v>
-                </c:pt>
-                <c:pt idx="359">
-                  <c:v>1348</c:v>
-                </c:pt>
-                <c:pt idx="360">
-                  <c:v>1437</c:v>
-                </c:pt>
-                <c:pt idx="361">
-                  <c:v>1366</c:v>
-                </c:pt>
-                <c:pt idx="362">
-                  <c:v>1325</c:v>
-                </c:pt>
-                <c:pt idx="363">
-                  <c:v>1238</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6769-40B7-B94F-63D502BCD70A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Figure 49. Daily excess deaths'!$H$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>29/12/2020</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Figure 49. Daily excess deaths'!$B$9:$B$395</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="387"/>
-                <c:pt idx="0">
-                  <c:v>43831</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43832</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43833</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43834</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43835</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43836</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43837</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43838</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43839</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43840</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43841</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43842</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43843</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>43844</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>43845</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>43846</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>43847</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>43848</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>43849</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43850</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>43851</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>43852</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>43853</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>43854</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>43855</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>43856</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>43857</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>43858</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>43859</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>43860</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>43861</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>43862</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>43863</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>43864</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>43865</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>43866</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>43867</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>43868</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>43869</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>43870</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>43871</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>43872</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>43873</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>43874</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>43875</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>43876</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>43877</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>43878</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>43879</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>43880</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>43881</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>43882</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>43883</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>43884</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>43885</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>43886</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>43887</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>43888</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>43889</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>43890</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>43891</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>43892</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>43893</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>43894</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>43895</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>43896</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>43897</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>43898</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>43899</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>43900</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>43901</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>43902</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>43903</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>43904</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>43905</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>43906</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>43907</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>43908</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>43909</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>43910</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>43911</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>43912</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>43913</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>43914</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>43915</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>43916</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>43917</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>43918</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>43919</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>43920</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>43921</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>43922</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>43923</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>43924</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>43925</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>43926</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>43927</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>43928</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>43929</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>43930</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>43931</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>43932</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>43933</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>43934</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>43935</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>43936</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>43937</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>43938</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>43939</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>43940</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>43941</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>43942</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>43943</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>43944</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>43945</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>43946</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>43947</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>43948</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>43949</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>43950</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>43951</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>43952</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>43953</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>43954</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>43955</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>43956</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>43957</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>43958</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>43959</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>43960</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>43961</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>43962</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>43963</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>43964</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>43965</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>43966</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>43967</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>43968</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>43969</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>43970</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>43971</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>43972</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>43973</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>43974</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>43975</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>43976</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>43977</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>43978</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>43979</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>43980</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>43981</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>43982</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>43983</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>43984</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>43985</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>43986</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>43987</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>43988</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>43989</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>43990</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>43991</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>43992</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>43993</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>43994</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>43995</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>43996</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>43997</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>43998</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>43999</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>44000</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>44001</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>44002</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>44003</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>44004</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>44005</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>44006</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>44007</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>44008</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>44009</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>44010</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>44011</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>44012</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>44013</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>44014</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>44015</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>44016</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>44017</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>44018</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>44019</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>44020</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>44021</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>44022</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>44023</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>44024</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>44025</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>44026</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>44027</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>44028</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>44029</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>44030</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>44031</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>44032</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>44033</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>44034</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>44035</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>44036</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>44037</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>44038</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>44039</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>44040</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>44041</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>44042</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>44043</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>44044</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>44045</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>44046</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>44047</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>44048</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>44049</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>44050</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>44051</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>44052</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>44053</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>44054</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>44055</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>44056</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>44057</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>44058</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>44059</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>44060</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>44061</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>44062</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>44063</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>44064</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>44065</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>44066</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>44067</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>44068</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>44069</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>44070</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>44071</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>44072</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>44073</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>44074</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>44075</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>44076</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>44077</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>44078</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>44079</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>44080</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>44081</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>44082</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>44083</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>44084</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>44085</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>44086</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>44087</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>44088</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>44089</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>44090</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>44091</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>44092</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>44093</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>44094</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>44095</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>44096</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>44097</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>44098</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>44099</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>44100</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>44101</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>44102</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>44103</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>44104</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>44105</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>44106</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>44107</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>44108</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>44109</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>44110</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>44111</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>44112</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>44113</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>44114</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>44115</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>44116</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>44117</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>44118</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>44119</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>44120</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>44121</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>44122</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>44123</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>44124</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>44125</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>44126</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>44127</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>44128</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>44129</c:v>
-                </c:pt>
-                <c:pt idx="299">
-                  <c:v>44130</c:v>
-                </c:pt>
-                <c:pt idx="300">
-                  <c:v>44131</c:v>
-                </c:pt>
-                <c:pt idx="301">
-                  <c:v>44132</c:v>
-                </c:pt>
-                <c:pt idx="302">
-                  <c:v>44133</c:v>
-                </c:pt>
-                <c:pt idx="303">
-                  <c:v>44134</c:v>
-                </c:pt>
-                <c:pt idx="304">
-                  <c:v>44135</c:v>
-                </c:pt>
-                <c:pt idx="305">
-                  <c:v>44136</c:v>
-                </c:pt>
-                <c:pt idx="306">
-                  <c:v>44137</c:v>
-                </c:pt>
-                <c:pt idx="307">
-                  <c:v>44138</c:v>
-                </c:pt>
-                <c:pt idx="308">
-                  <c:v>44139</c:v>
-                </c:pt>
-                <c:pt idx="309">
-                  <c:v>44140</c:v>
-                </c:pt>
-                <c:pt idx="310">
-                  <c:v>44141</c:v>
-                </c:pt>
-                <c:pt idx="311">
-                  <c:v>44142</c:v>
-                </c:pt>
-                <c:pt idx="312">
-                  <c:v>44143</c:v>
-                </c:pt>
-                <c:pt idx="313">
-                  <c:v>44144</c:v>
-                </c:pt>
-                <c:pt idx="314">
-                  <c:v>44145</c:v>
-                </c:pt>
-                <c:pt idx="315">
-                  <c:v>44146</c:v>
-                </c:pt>
-                <c:pt idx="316">
-                  <c:v>44147</c:v>
-                </c:pt>
-                <c:pt idx="317">
-                  <c:v>44148</c:v>
-                </c:pt>
-                <c:pt idx="318">
-                  <c:v>44149</c:v>
-                </c:pt>
-                <c:pt idx="319">
-                  <c:v>44150</c:v>
-                </c:pt>
-                <c:pt idx="320">
-                  <c:v>44151</c:v>
-                </c:pt>
-                <c:pt idx="321">
-                  <c:v>44152</c:v>
-                </c:pt>
-                <c:pt idx="322">
-                  <c:v>44153</c:v>
-                </c:pt>
-                <c:pt idx="323">
-                  <c:v>44154</c:v>
-                </c:pt>
-                <c:pt idx="324">
-                  <c:v>44155</c:v>
-                </c:pt>
-                <c:pt idx="325">
-                  <c:v>44156</c:v>
-                </c:pt>
-                <c:pt idx="326">
-                  <c:v>44157</c:v>
-                </c:pt>
-                <c:pt idx="327">
-                  <c:v>44158</c:v>
-                </c:pt>
-                <c:pt idx="328">
-                  <c:v>44159</c:v>
-                </c:pt>
-                <c:pt idx="329">
-                  <c:v>44160</c:v>
-                </c:pt>
-                <c:pt idx="330">
-                  <c:v>44161</c:v>
-                </c:pt>
-                <c:pt idx="331">
-                  <c:v>44162</c:v>
-                </c:pt>
-                <c:pt idx="332">
-                  <c:v>44163</c:v>
-                </c:pt>
-                <c:pt idx="333">
-                  <c:v>44164</c:v>
-                </c:pt>
-                <c:pt idx="334">
-                  <c:v>44165</c:v>
-                </c:pt>
-                <c:pt idx="335">
-                  <c:v>44166</c:v>
-                </c:pt>
-                <c:pt idx="336">
-                  <c:v>44167</c:v>
-                </c:pt>
-                <c:pt idx="337">
-                  <c:v>44168</c:v>
-                </c:pt>
-                <c:pt idx="338">
-                  <c:v>44169</c:v>
-                </c:pt>
-                <c:pt idx="339">
-                  <c:v>44170</c:v>
-                </c:pt>
-                <c:pt idx="340">
-                  <c:v>44171</c:v>
-                </c:pt>
-                <c:pt idx="341">
-                  <c:v>44172</c:v>
-                </c:pt>
-                <c:pt idx="342">
-                  <c:v>44173</c:v>
-                </c:pt>
-                <c:pt idx="343">
-                  <c:v>44174</c:v>
-                </c:pt>
-                <c:pt idx="344">
-                  <c:v>44175</c:v>
-                </c:pt>
-                <c:pt idx="345">
-                  <c:v>44176</c:v>
-                </c:pt>
-                <c:pt idx="346">
-                  <c:v>44177</c:v>
-                </c:pt>
-                <c:pt idx="347">
-                  <c:v>44178</c:v>
-                </c:pt>
-                <c:pt idx="348">
-                  <c:v>44179</c:v>
-                </c:pt>
-                <c:pt idx="349">
-                  <c:v>44180</c:v>
-                </c:pt>
-                <c:pt idx="350">
-                  <c:v>44181</c:v>
-                </c:pt>
-                <c:pt idx="351">
-                  <c:v>44182</c:v>
-                </c:pt>
-                <c:pt idx="352">
-                  <c:v>44183</c:v>
-                </c:pt>
-                <c:pt idx="353">
-                  <c:v>44184</c:v>
-                </c:pt>
-                <c:pt idx="354">
-                  <c:v>44185</c:v>
-                </c:pt>
-                <c:pt idx="355">
-                  <c:v>44186</c:v>
-                </c:pt>
-                <c:pt idx="356">
-                  <c:v>44187</c:v>
-                </c:pt>
-                <c:pt idx="357">
-                  <c:v>44188</c:v>
-                </c:pt>
-                <c:pt idx="358">
-                  <c:v>44189</c:v>
-                </c:pt>
-                <c:pt idx="359">
-                  <c:v>44190</c:v>
-                </c:pt>
-                <c:pt idx="360">
-                  <c:v>44191</c:v>
-                </c:pt>
-                <c:pt idx="361">
-                  <c:v>44192</c:v>
-                </c:pt>
-                <c:pt idx="362">
-                  <c:v>44193</c:v>
-                </c:pt>
-                <c:pt idx="363">
-                  <c:v>44194</c:v>
-                </c:pt>
-                <c:pt idx="364">
-                  <c:v>44195</c:v>
-                </c:pt>
-                <c:pt idx="365">
-                  <c:v>44196</c:v>
-                </c:pt>
-                <c:pt idx="366">
-                  <c:v>44197</c:v>
-                </c:pt>
-                <c:pt idx="367">
-                  <c:v>44198</c:v>
-                </c:pt>
-                <c:pt idx="368">
-                  <c:v>44199</c:v>
-                </c:pt>
-                <c:pt idx="369">
-                  <c:v>44200</c:v>
-                </c:pt>
-                <c:pt idx="370">
-                  <c:v>44201</c:v>
-                </c:pt>
-                <c:pt idx="371">
-                  <c:v>44202</c:v>
-                </c:pt>
-                <c:pt idx="372">
-                  <c:v>44203</c:v>
-                </c:pt>
-                <c:pt idx="373">
-                  <c:v>44204</c:v>
-                </c:pt>
-                <c:pt idx="374">
-                  <c:v>44205</c:v>
-                </c:pt>
-                <c:pt idx="375">
-                  <c:v>44206</c:v>
-                </c:pt>
-                <c:pt idx="376">
-                  <c:v>44207</c:v>
-                </c:pt>
-                <c:pt idx="377">
-                  <c:v>44208</c:v>
-                </c:pt>
-                <c:pt idx="378">
-                  <c:v>44209</c:v>
-                </c:pt>
-                <c:pt idx="379">
-                  <c:v>44210</c:v>
-                </c:pt>
-                <c:pt idx="380">
-                  <c:v>44211</c:v>
-                </c:pt>
-                <c:pt idx="381">
-                  <c:v>44212</c:v>
-                </c:pt>
-                <c:pt idx="382">
-                  <c:v>44213</c:v>
-                </c:pt>
-                <c:pt idx="383">
-                  <c:v>44214</c:v>
-                </c:pt>
-                <c:pt idx="384">
-                  <c:v>44215</c:v>
-                </c:pt>
-                <c:pt idx="385">
-                  <c:v>44216</c:v>
-                </c:pt>
-                <c:pt idx="386">
-                  <c:v>44217</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
               <c:f>'Figure 49. Daily excess deaths'!$H$9:$H$372</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
@@ -4998,7 +2717,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>'Figure 49. Daily excess deaths'!$J$8</c:f>
@@ -7346,2129 +5065,8 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Figure 49. Daily excess deaths'!$K$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>diff</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Figure 49. Daily excess deaths'!$B$9:$B$395</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="387"/>
-                <c:pt idx="0">
-                  <c:v>43831</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43832</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43833</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43834</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43835</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43836</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43837</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43838</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43839</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43840</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43841</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43842</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43843</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>43844</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>43845</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>43846</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>43847</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>43848</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>43849</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43850</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>43851</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>43852</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>43853</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>43854</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>43855</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>43856</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>43857</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>43858</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>43859</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>43860</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>43861</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>43862</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>43863</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>43864</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>43865</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>43866</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>43867</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>43868</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>43869</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>43870</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>43871</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>43872</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>43873</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>43874</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>43875</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>43876</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>43877</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>43878</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>43879</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>43880</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>43881</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>43882</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>43883</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>43884</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>43885</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>43886</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>43887</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>43888</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>43889</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>43890</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>43891</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>43892</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>43893</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>43894</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>43895</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>43896</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>43897</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>43898</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>43899</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>43900</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>43901</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>43902</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>43903</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>43904</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>43905</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>43906</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>43907</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>43908</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>43909</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>43910</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>43911</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>43912</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>43913</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>43914</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>43915</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>43916</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>43917</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>43918</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>43919</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>43920</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>43921</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>43922</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>43923</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>43924</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>43925</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>43926</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>43927</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>43928</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>43929</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>43930</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>43931</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>43932</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>43933</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>43934</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>43935</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>43936</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>43937</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>43938</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>43939</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>43940</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>43941</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>43942</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>43943</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>43944</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>43945</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>43946</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>43947</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>43948</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>43949</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>43950</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>43951</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>43952</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>43953</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>43954</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>43955</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>43956</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>43957</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>43958</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>43959</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>43960</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>43961</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>43962</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>43963</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>43964</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>43965</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>43966</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>43967</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>43968</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>43969</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>43970</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>43971</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>43972</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>43973</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>43974</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>43975</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>43976</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>43977</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>43978</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>43979</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>43980</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>43981</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>43982</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>43983</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>43984</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>43985</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>43986</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>43987</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>43988</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>43989</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>43990</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>43991</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>43992</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>43993</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>43994</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>43995</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>43996</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>43997</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>43998</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>43999</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>44000</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>44001</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>44002</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>44003</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>44004</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>44005</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>44006</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>44007</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>44008</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>44009</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>44010</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>44011</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>44012</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>44013</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>44014</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>44015</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>44016</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>44017</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>44018</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>44019</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>44020</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>44021</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>44022</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>44023</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>44024</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>44025</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>44026</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>44027</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>44028</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>44029</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>44030</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>44031</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>44032</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>44033</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>44034</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>44035</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>44036</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>44037</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>44038</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>44039</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>44040</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>44041</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>44042</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>44043</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>44044</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>44045</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>44046</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>44047</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>44048</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>44049</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>44050</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>44051</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>44052</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>44053</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>44054</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>44055</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>44056</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>44057</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>44058</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>44059</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>44060</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>44061</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>44062</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>44063</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>44064</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>44065</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>44066</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>44067</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>44068</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>44069</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>44070</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>44071</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>44072</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>44073</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>44074</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>44075</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>44076</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>44077</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>44078</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>44079</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>44080</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>44081</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>44082</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>44083</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>44084</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>44085</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>44086</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>44087</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>44088</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>44089</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>44090</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>44091</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>44092</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>44093</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>44094</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>44095</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>44096</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>44097</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>44098</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>44099</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>44100</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>44101</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>44102</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>44103</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>44104</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>44105</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>44106</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>44107</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>44108</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>44109</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>44110</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>44111</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>44112</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>44113</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>44114</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>44115</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>44116</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>44117</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>44118</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>44119</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>44120</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>44121</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>44122</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>44123</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>44124</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>44125</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>44126</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>44127</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>44128</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>44129</c:v>
-                </c:pt>
-                <c:pt idx="299">
-                  <c:v>44130</c:v>
-                </c:pt>
-                <c:pt idx="300">
-                  <c:v>44131</c:v>
-                </c:pt>
-                <c:pt idx="301">
-                  <c:v>44132</c:v>
-                </c:pt>
-                <c:pt idx="302">
-                  <c:v>44133</c:v>
-                </c:pt>
-                <c:pt idx="303">
-                  <c:v>44134</c:v>
-                </c:pt>
-                <c:pt idx="304">
-                  <c:v>44135</c:v>
-                </c:pt>
-                <c:pt idx="305">
-                  <c:v>44136</c:v>
-                </c:pt>
-                <c:pt idx="306">
-                  <c:v>44137</c:v>
-                </c:pt>
-                <c:pt idx="307">
-                  <c:v>44138</c:v>
-                </c:pt>
-                <c:pt idx="308">
-                  <c:v>44139</c:v>
-                </c:pt>
-                <c:pt idx="309">
-                  <c:v>44140</c:v>
-                </c:pt>
-                <c:pt idx="310">
-                  <c:v>44141</c:v>
-                </c:pt>
-                <c:pt idx="311">
-                  <c:v>44142</c:v>
-                </c:pt>
-                <c:pt idx="312">
-                  <c:v>44143</c:v>
-                </c:pt>
-                <c:pt idx="313">
-                  <c:v>44144</c:v>
-                </c:pt>
-                <c:pt idx="314">
-                  <c:v>44145</c:v>
-                </c:pt>
-                <c:pt idx="315">
-                  <c:v>44146</c:v>
-                </c:pt>
-                <c:pt idx="316">
-                  <c:v>44147</c:v>
-                </c:pt>
-                <c:pt idx="317">
-                  <c:v>44148</c:v>
-                </c:pt>
-                <c:pt idx="318">
-                  <c:v>44149</c:v>
-                </c:pt>
-                <c:pt idx="319">
-                  <c:v>44150</c:v>
-                </c:pt>
-                <c:pt idx="320">
-                  <c:v>44151</c:v>
-                </c:pt>
-                <c:pt idx="321">
-                  <c:v>44152</c:v>
-                </c:pt>
-                <c:pt idx="322">
-                  <c:v>44153</c:v>
-                </c:pt>
-                <c:pt idx="323">
-                  <c:v>44154</c:v>
-                </c:pt>
-                <c:pt idx="324">
-                  <c:v>44155</c:v>
-                </c:pt>
-                <c:pt idx="325">
-                  <c:v>44156</c:v>
-                </c:pt>
-                <c:pt idx="326">
-                  <c:v>44157</c:v>
-                </c:pt>
-                <c:pt idx="327">
-                  <c:v>44158</c:v>
-                </c:pt>
-                <c:pt idx="328">
-                  <c:v>44159</c:v>
-                </c:pt>
-                <c:pt idx="329">
-                  <c:v>44160</c:v>
-                </c:pt>
-                <c:pt idx="330">
-                  <c:v>44161</c:v>
-                </c:pt>
-                <c:pt idx="331">
-                  <c:v>44162</c:v>
-                </c:pt>
-                <c:pt idx="332">
-                  <c:v>44163</c:v>
-                </c:pt>
-                <c:pt idx="333">
-                  <c:v>44164</c:v>
-                </c:pt>
-                <c:pt idx="334">
-                  <c:v>44165</c:v>
-                </c:pt>
-                <c:pt idx="335">
-                  <c:v>44166</c:v>
-                </c:pt>
-                <c:pt idx="336">
-                  <c:v>44167</c:v>
-                </c:pt>
-                <c:pt idx="337">
-                  <c:v>44168</c:v>
-                </c:pt>
-                <c:pt idx="338">
-                  <c:v>44169</c:v>
-                </c:pt>
-                <c:pt idx="339">
-                  <c:v>44170</c:v>
-                </c:pt>
-                <c:pt idx="340">
-                  <c:v>44171</c:v>
-                </c:pt>
-                <c:pt idx="341">
-                  <c:v>44172</c:v>
-                </c:pt>
-                <c:pt idx="342">
-                  <c:v>44173</c:v>
-                </c:pt>
-                <c:pt idx="343">
-                  <c:v>44174</c:v>
-                </c:pt>
-                <c:pt idx="344">
-                  <c:v>44175</c:v>
-                </c:pt>
-                <c:pt idx="345">
-                  <c:v>44176</c:v>
-                </c:pt>
-                <c:pt idx="346">
-                  <c:v>44177</c:v>
-                </c:pt>
-                <c:pt idx="347">
-                  <c:v>44178</c:v>
-                </c:pt>
-                <c:pt idx="348">
-                  <c:v>44179</c:v>
-                </c:pt>
-                <c:pt idx="349">
-                  <c:v>44180</c:v>
-                </c:pt>
-                <c:pt idx="350">
-                  <c:v>44181</c:v>
-                </c:pt>
-                <c:pt idx="351">
-                  <c:v>44182</c:v>
-                </c:pt>
-                <c:pt idx="352">
-                  <c:v>44183</c:v>
-                </c:pt>
-                <c:pt idx="353">
-                  <c:v>44184</c:v>
-                </c:pt>
-                <c:pt idx="354">
-                  <c:v>44185</c:v>
-                </c:pt>
-                <c:pt idx="355">
-                  <c:v>44186</c:v>
-                </c:pt>
-                <c:pt idx="356">
-                  <c:v>44187</c:v>
-                </c:pt>
-                <c:pt idx="357">
-                  <c:v>44188</c:v>
-                </c:pt>
-                <c:pt idx="358">
-                  <c:v>44189</c:v>
-                </c:pt>
-                <c:pt idx="359">
-                  <c:v>44190</c:v>
-                </c:pt>
-                <c:pt idx="360">
-                  <c:v>44191</c:v>
-                </c:pt>
-                <c:pt idx="361">
-                  <c:v>44192</c:v>
-                </c:pt>
-                <c:pt idx="362">
-                  <c:v>44193</c:v>
-                </c:pt>
-                <c:pt idx="363">
-                  <c:v>44194</c:v>
-                </c:pt>
-                <c:pt idx="364">
-                  <c:v>44195</c:v>
-                </c:pt>
-                <c:pt idx="365">
-                  <c:v>44196</c:v>
-                </c:pt>
-                <c:pt idx="366">
-                  <c:v>44197</c:v>
-                </c:pt>
-                <c:pt idx="367">
-                  <c:v>44198</c:v>
-                </c:pt>
-                <c:pt idx="368">
-                  <c:v>44199</c:v>
-                </c:pt>
-                <c:pt idx="369">
-                  <c:v>44200</c:v>
-                </c:pt>
-                <c:pt idx="370">
-                  <c:v>44201</c:v>
-                </c:pt>
-                <c:pt idx="371">
-                  <c:v>44202</c:v>
-                </c:pt>
-                <c:pt idx="372">
-                  <c:v>44203</c:v>
-                </c:pt>
-                <c:pt idx="373">
-                  <c:v>44204</c:v>
-                </c:pt>
-                <c:pt idx="374">
-                  <c:v>44205</c:v>
-                </c:pt>
-                <c:pt idx="375">
-                  <c:v>44206</c:v>
-                </c:pt>
-                <c:pt idx="376">
-                  <c:v>44207</c:v>
-                </c:pt>
-                <c:pt idx="377">
-                  <c:v>44208</c:v>
-                </c:pt>
-                <c:pt idx="378">
-                  <c:v>44209</c:v>
-                </c:pt>
-                <c:pt idx="379">
-                  <c:v>44210</c:v>
-                </c:pt>
-                <c:pt idx="380">
-                  <c:v>44211</c:v>
-                </c:pt>
-                <c:pt idx="381">
-                  <c:v>44212</c:v>
-                </c:pt>
-                <c:pt idx="382">
-                  <c:v>44213</c:v>
-                </c:pt>
-                <c:pt idx="383">
-                  <c:v>44214</c:v>
-                </c:pt>
-                <c:pt idx="384">
-                  <c:v>44215</c:v>
-                </c:pt>
-                <c:pt idx="385">
-                  <c:v>44216</c:v>
-                </c:pt>
-                <c:pt idx="386">
-                  <c:v>44217</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Figure 49. Daily excess deaths'!$L$9:$L$372</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="364"/>
-                <c:pt idx="61">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>102</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>117</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>154</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>173</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>219</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>278</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>336</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>374</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>384</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>465</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>539</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>603</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>698</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>731</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>743</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>838</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>830</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>804</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>912</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>975</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>875</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>850</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>862</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>858</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>804</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>771</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>784</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>752</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>744</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>706</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>685</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>685</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>649</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>644</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>593</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>603</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>556</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>561</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>506</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>498</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>493</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>484</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>479</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>424</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>387</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>412</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>391</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>392</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>330</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>330</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>275</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>255</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>277</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>269</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>268</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>253</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>231</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>234</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>201</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>195</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>199</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>169</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>176</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>188</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>171</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>182</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>163</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>122</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>156</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>121</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>109</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>111</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>103</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>124</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>123</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>159</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>171</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>192</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>185</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>188</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>171</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>204</c:v>
-                </c:pt>
-                <c:pt idx="299">
-                  <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="300">
-                  <c:v>218</c:v>
-                </c:pt>
-                <c:pt idx="301">
-                  <c:v>238</c:v>
-                </c:pt>
-                <c:pt idx="302">
-                  <c:v>249</c:v>
-                </c:pt>
-                <c:pt idx="303">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="304">
-                  <c:v>276</c:v>
-                </c:pt>
-                <c:pt idx="305">
-                  <c:v>286</c:v>
-                </c:pt>
-                <c:pt idx="306">
-                  <c:v>281</c:v>
-                </c:pt>
-                <c:pt idx="307">
-                  <c:v>292</c:v>
-                </c:pt>
-                <c:pt idx="308">
-                  <c:v>278</c:v>
-                </c:pt>
-                <c:pt idx="309">
-                  <c:v>301</c:v>
-                </c:pt>
-                <c:pt idx="310">
-                  <c:v>334</c:v>
-                </c:pt>
-                <c:pt idx="311">
-                  <c:v>332</c:v>
-                </c:pt>
-                <c:pt idx="312">
-                  <c:v>340</c:v>
-                </c:pt>
-                <c:pt idx="313">
-                  <c:v>403</c:v>
-                </c:pt>
-                <c:pt idx="314">
-                  <c:v>318</c:v>
-                </c:pt>
-                <c:pt idx="315">
-                  <c:v>310</c:v>
-                </c:pt>
-                <c:pt idx="316">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="317">
-                  <c:v>358</c:v>
-                </c:pt>
-                <c:pt idx="318">
-                  <c:v>357</c:v>
-                </c:pt>
-                <c:pt idx="319">
-                  <c:v>380</c:v>
-                </c:pt>
-                <c:pt idx="320">
-                  <c:v>359</c:v>
-                </c:pt>
-                <c:pt idx="321">
-                  <c:v>363</c:v>
-                </c:pt>
-                <c:pt idx="322">
-                  <c:v>436</c:v>
-                </c:pt>
-                <c:pt idx="323">
-                  <c:v>397</c:v>
-                </c:pt>
-                <c:pt idx="324">
-                  <c:v>388</c:v>
-                </c:pt>
-                <c:pt idx="325">
-                  <c:v>396</c:v>
-                </c:pt>
-                <c:pt idx="326">
-                  <c:v>406</c:v>
-                </c:pt>
-                <c:pt idx="327">
-                  <c:v>399</c:v>
-                </c:pt>
-                <c:pt idx="328">
-                  <c:v>402</c:v>
-                </c:pt>
-                <c:pt idx="329">
-                  <c:v>423</c:v>
-                </c:pt>
-                <c:pt idx="330">
-                  <c:v>372</c:v>
-                </c:pt>
-                <c:pt idx="331">
-                  <c:v>359</c:v>
-                </c:pt>
-                <c:pt idx="332">
-                  <c:v>379</c:v>
-                </c:pt>
-                <c:pt idx="333">
-                  <c:v>401</c:v>
-                </c:pt>
-                <c:pt idx="334">
-                  <c:v>361</c:v>
-                </c:pt>
-                <c:pt idx="335">
-                  <c:v>349</c:v>
-                </c:pt>
-                <c:pt idx="336">
-                  <c:v>337</c:v>
-                </c:pt>
-                <c:pt idx="337">
-                  <c:v>403</c:v>
-                </c:pt>
-                <c:pt idx="338">
-                  <c:v>413</c:v>
-                </c:pt>
-                <c:pt idx="339">
-                  <c:v>340</c:v>
-                </c:pt>
-                <c:pt idx="340">
-                  <c:v>351</c:v>
-                </c:pt>
-                <c:pt idx="341">
-                  <c:v>354</c:v>
-                </c:pt>
-                <c:pt idx="342">
-                  <c:v>375</c:v>
-                </c:pt>
-                <c:pt idx="343">
-                  <c:v>373</c:v>
-                </c:pt>
-                <c:pt idx="344">
-                  <c:v>373</c:v>
-                </c:pt>
-                <c:pt idx="345">
-                  <c:v>397</c:v>
-                </c:pt>
-                <c:pt idx="346">
-                  <c:v>374</c:v>
-                </c:pt>
-                <c:pt idx="347">
-                  <c:v>364</c:v>
-                </c:pt>
-                <c:pt idx="348">
-                  <c:v>410</c:v>
-                </c:pt>
-                <c:pt idx="349">
-                  <c:v>385</c:v>
-                </c:pt>
-                <c:pt idx="350">
-                  <c:v>357</c:v>
-                </c:pt>
-                <c:pt idx="351">
-                  <c:v>433</c:v>
-                </c:pt>
-                <c:pt idx="352">
-                  <c:v>434</c:v>
-                </c:pt>
-                <c:pt idx="353">
-                  <c:v>407</c:v>
-                </c:pt>
-                <c:pt idx="354">
-                  <c:v>428</c:v>
-                </c:pt>
-                <c:pt idx="355">
-                  <c:v>492</c:v>
-                </c:pt>
-                <c:pt idx="356">
-                  <c:v>491</c:v>
-                </c:pt>
-                <c:pt idx="357">
-                  <c:v>481</c:v>
-                </c:pt>
-                <c:pt idx="358">
-                  <c:v>479</c:v>
-                </c:pt>
-                <c:pt idx="359">
-                  <c:v>534</c:v>
-                </c:pt>
-                <c:pt idx="360">
-                  <c:v>564</c:v>
-                </c:pt>
-                <c:pt idx="361">
-                  <c:v>568</c:v>
-                </c:pt>
-                <c:pt idx="362">
-                  <c:v>585</c:v>
-                </c:pt>
-                <c:pt idx="363">
-                  <c:v>581</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-6769-40B7-B94F-63D502BCD70A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>'Figure 49. Daily excess deaths'!$D$8</c:f>
@@ -11898,7 +7496,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12919,9 +8517,9 @@
   <dimension ref="B1:L395"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A365" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C7" sqref="C7"/>
-      <selection pane="bottomLeft" activeCell="J376" sqref="J376:J382"/>
+      <selection pane="bottomLeft" activeCell="K107" sqref="K107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23403,7 +19001,7 @@
         <v>1584.5340000000001</v>
       </c>
       <c r="K329" s="19">
-        <f t="shared" ref="K329:K392" si="5">J329-C329</f>
+        <f t="shared" ref="K329:K372" si="5">J329-C329</f>
         <v>110.53400000000011</v>
       </c>
       <c r="L329">
@@ -25165,7 +20763,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>